<commit_message>
Updated code on timestamp:   16-06-2022 - 12:35:29.68
</commit_message>
<xml_diff>
--- a/S30 Curriculum_my.xlsx
+++ b/S30 Curriculum_my.xlsx
@@ -409,7 +409,7 @@
         <v>Design-1</v>
       </c>
       <c r="D2" t="str">
-        <v>leet 706</v>
+        <v>706</v>
       </c>
     </row>
     <row r="3">
@@ -421,6 +421,9 @@
       </c>
       <c r="C3" t="str">
         <v>Design-1</v>
+      </c>
+      <c r="D3" t="str">
+        <v>155</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Updated code on timestamp:   16-06-2022 - 12:43:17.55
</commit_message>
<xml_diff>
--- a/S30 Curriculum_my.xlsx
+++ b/S30 Curriculum_my.xlsx
@@ -1638,6 +1638,9 @@
       <c r="C119" t="str">
         <v>Array-3</v>
       </c>
+      <c r="D119" t="str">
+        <v>274 275</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
@@ -1649,6 +1652,9 @@
       <c r="C120" t="str">
         <v>Array-3</v>
       </c>
+      <c r="D120" t="str">
+        <v>42 407</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
@@ -1660,6 +1666,9 @@
       <c r="C121" t="str">
         <v>Array-3</v>
       </c>
+      <c r="D121" t="str">
+        <v>189</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="str">
@@ -1671,6 +1680,9 @@
       <c r="C122" t="str">
         <v>Array-4</v>
       </c>
+      <c r="D122" t="str">
+        <v>561</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
@@ -1682,6 +1694,9 @@
       <c r="C123" t="str">
         <v>Array-4</v>
       </c>
+      <c r="D123" t="str">
+        <v>53</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
@@ -1693,6 +1708,9 @@
       <c r="C124" t="str">
         <v>Array-4</v>
       </c>
+      <c r="D124" t="str">
+        <v>31</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="str">
@@ -1726,6 +1744,9 @@
       <c r="C127" t="str">
         <v>Design-7</v>
       </c>
+      <c r="D127" t="str">
+        <v>460</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="str">
@@ -1783,6 +1804,9 @@
       <c r="C133" t="str">
         <v>Stack-1</v>
       </c>
+      <c r="D133" t="str">
+        <v>503</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="str">
@@ -1794,6 +1818,9 @@
       <c r="C134" t="str">
         <v>Stack-2</v>
       </c>
+      <c r="D134" t="str">
+        <v>636</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="str">
@@ -1838,6 +1865,9 @@
       <c r="C138" t="str">
         <v>Greedy-2</v>
       </c>
+      <c r="D138" t="str">
+        <v>575</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="str">
@@ -1849,6 +1879,9 @@
       <c r="C139" t="str">
         <v>Greedy-2</v>
       </c>
+      <c r="D139" t="str">
+        <v>621</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="str">
@@ -1859,6 +1892,9 @@
       </c>
       <c r="C140" t="str">
         <v>Greedy-3</v>
+      </c>
+      <c r="D140" t="str">
+        <v>406</v>
       </c>
     </row>
     <row r="141">

</xml_diff>

<commit_message>
Updated code on timestamp:   16-06-2022 - 12:50:14.60
</commit_message>
<xml_diff>
--- a/S30 Curriculum_my.xlsx
+++ b/S30 Curriculum_my.xlsx
@@ -1942,6 +1942,9 @@
       <c r="C145" t="str">
         <v>BFS-3</v>
       </c>
+      <c r="D145" t="str">
+        <v>301</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="str">
@@ -1953,6 +1956,9 @@
       <c r="C146" t="str">
         <v>BFS-3</v>
       </c>
+      <c r="D146" t="str">
+        <v>133</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="str">
@@ -1964,6 +1970,9 @@
       <c r="C147" t="str">
         <v>BFS-4</v>
       </c>
+      <c r="D147" t="str">
+        <v>529</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="str">
@@ -1975,6 +1984,9 @@
       <c r="C148" t="str">
         <v>BFS-4</v>
       </c>
+      <c r="D148" t="str">
+        <v>909</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="str">
@@ -1986,6 +1998,9 @@
       <c r="C149" t="str">
         <v>DP-7</v>
       </c>
+      <c r="D149" t="str">
+        <v>72</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="str">
@@ -1997,6 +2012,9 @@
       <c r="C150" t="str">
         <v>DP-7</v>
       </c>
+      <c r="D150" t="str">
+        <v>10</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="str">
@@ -2008,6 +2026,9 @@
       <c r="C151" t="str">
         <v>DP-8</v>
       </c>
+      <c r="D151" t="str">
+        <v>413</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="str">
@@ -2030,6 +2051,9 @@
       <c r="C153" t="str">
         <v>DP-9</v>
       </c>
+      <c r="D153" t="str">
+        <v>300</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="str">
@@ -2041,6 +2065,9 @@
       <c r="C154" t="str">
         <v>DP-9</v>
       </c>
+      <c r="D154" t="str">
+        <v>354</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="str">
@@ -2068,6 +2095,9 @@
       <c r="C157" t="str">
         <v>DP-10</v>
       </c>
+      <c r="D157" t="str">
+        <v>887</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="str">
@@ -2079,6 +2109,9 @@
       <c r="C158" t="str">
         <v>DP-10</v>
       </c>
+      <c r="D158" t="str">
+        <v>312</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="str">
@@ -2090,6 +2123,9 @@
       <c r="C159" t="str">
         <v>Graph-2</v>
       </c>
+      <c r="D159" t="str">
+        <v>1192</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="str">
@@ -2101,6 +2137,9 @@
       <c r="C160" t="str">
         <v>Graph-2</v>
       </c>
+      <c r="D160" t="str">
+        <v>924 928</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="str">
@@ -2123,6 +2162,9 @@
       <c r="C162" t="str">
         <v>Backtracking-4</v>
       </c>
+      <c r="D162" t="str">
+        <v>1096</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="str">
@@ -2145,6 +2187,9 @@
       <c r="C164" t="str">
         <v>Greedy-4</v>
       </c>
+      <c r="D164" t="str">
+        <v>1007</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="str">
@@ -2171,6 +2216,9 @@
       </c>
       <c r="C167" t="str">
         <v>Greedy-5</v>
+      </c>
+      <c r="D167" t="str">
+        <v>44</v>
       </c>
     </row>
     <row r="168">

</xml_diff>